<commit_message>
Add more details to wastewater metadata
</commit_message>
<xml_diff>
--- a/input/activity/wastewater/UN_Percentage_WW_Treatment.xlsx
+++ b/input/activity/wastewater/UN_Percentage_WW_Treatment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="2680" windowWidth="25600" windowHeight="14300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="107">
   <si>
     <t>country</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t>Source</t>
+  </si>
+  <si>
+    <t>http://unstats.un.org/unsd/environment/wastewater.htm</t>
   </si>
 </sst>
 </file>
@@ -386,20 +389,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -733,7 +738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -2418,10 +2423,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2444,6 +2449,11 @@
     <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>